<commit_message>
Implemented Golang code renderer for Gorm & sqlx
</commit_message>
<xml_diff>
--- a/docs/Store/Store example.xlsx
+++ b/docs/Store/Store example.xlsx
@@ -174,7 +174,7 @@
     <t>Modification data structure</t>
   </si>
   <si>
-    <t>modifications</t>
+    <t>modifications_table</t>
   </si>
   <si>
     <t>Embedded</t>
@@ -243,7 +243,7 @@
     <t>Address data structure</t>
   </si>
   <si>
-    <t>addresses</t>
+    <t>addresses_table</t>
   </si>
   <si>
     <t>First address line</t>
@@ -303,7 +303,7 @@
     <t>Analytics data structure</t>
   </si>
   <si>
-    <t>analyticses</t>
+    <t>analyticses_table</t>
   </si>
   <si>
     <t>PromotionId</t>
@@ -342,7 +342,7 @@
     <t>business_area_id</t>
   </si>
   <si>
-    <t>analyticses_promotion_id</t>
+    <t>analyticses_table_promotion_id</t>
   </si>
   <si>
     <t>Reference to Promotion</t>
@@ -351,7 +351,7 @@
     <t>ManyToOne</t>
   </si>
   <si>
-    <t>analytics_promotions</t>
+    <t>analytics_promotions_table</t>
   </si>
   <si>
     <t>Promotion</t>
@@ -363,25 +363,25 @@
     <t>id</t>
   </si>
   <si>
-    <t>analyticses_segment_id</t>
+    <t>analyticses_table_segment_id</t>
   </si>
   <si>
     <t>Reference to Segment</t>
   </si>
   <si>
-    <t>analytics_segments</t>
+    <t>analytics_segments_table</t>
   </si>
   <si>
     <t>Segment</t>
   </si>
   <si>
-    <t>analyticses_business_area_id</t>
+    <t>analyticses_table_business_area_id</t>
   </si>
   <si>
     <t>Reference to BusinessArea</t>
   </si>
   <si>
-    <t>analytics_business_areas</t>
+    <t>analytics_business_areas_table</t>
   </si>
   <si>
     <t>Business area</t>
@@ -396,7 +396,7 @@
     <t>client</t>
   </si>
   <si>
-    <t>client_clients</t>
+    <t>client_clients_table</t>
   </si>
   <si>
     <t>Table</t>
@@ -507,13 +507,13 @@
     <t>postal_postcode</t>
   </si>
   <si>
-    <t>client_clients_promotion_id</t>
-  </si>
-  <si>
-    <t>client_clients_segment_id</t>
-  </si>
-  <si>
-    <t>client_clients_business_area_id</t>
+    <t>client_clients_table_promotion_id</t>
+  </si>
+  <si>
+    <t>client_clients_table_segment_id</t>
+  </si>
+  <si>
+    <t>client_clients_table_business_area_id</t>
   </si>
   <si>
     <t>ClientAddress</t>
@@ -522,7 +522,7 @@
     <t>Client address</t>
   </si>
   <si>
-    <t>client_client_addresses</t>
+    <t>client_client_addresses_table</t>
   </si>
   <si>
     <t>AddressId</t>
@@ -540,13 +540,13 @@
     <t>client_id</t>
   </si>
   <si>
-    <t>client_client_addresses_client_id_id</t>
+    <t>client_client_addresses_table_client_id_id</t>
   </si>
   <si>
     <t>Unique clientId &amp; id</t>
   </si>
   <si>
-    <t>client_client_addresses_client_id</t>
+    <t>client_client_addresses_table_client_id</t>
   </si>
   <si>
     <t>Reference to client</t>
@@ -558,7 +558,7 @@
     <t>Order tables</t>
   </si>
   <si>
-    <t>order_orders</t>
+    <t>order_orders_table</t>
   </si>
   <si>
     <t>OrderId</t>
@@ -591,22 +591,22 @@
     <t>1</t>
   </si>
   <si>
-    <t>order_orders_client_id</t>
-  </si>
-  <si>
-    <t>order_orders_delivery_address_id</t>
+    <t>order_orders_table_client_id</t>
+  </si>
+  <si>
+    <t>order_orders_table_delivery_address_id</t>
   </si>
   <si>
     <t>Reference to address</t>
   </si>
   <si>
-    <t>order_orders_promotion_id</t>
-  </si>
-  <si>
-    <t>order_orders_segment_id</t>
-  </si>
-  <si>
-    <t>order_orders_business_area_id</t>
+    <t>order_orders_table_promotion_id</t>
+  </si>
+  <si>
+    <t>order_orders_table_segment_id</t>
+  </si>
+  <si>
+    <t>order_orders_table_business_area_id</t>
   </si>
   <si>
     <t>OrderLine</t>
@@ -615,7 +615,7 @@
     <t>Order line</t>
   </si>
   <si>
-    <t>order_order_lines</t>
+    <t>order_order_lines_table</t>
   </si>
   <si>
     <t>OrderLineId</t>
@@ -663,31 +663,31 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>order_order_lines_order_id</t>
+    <t>order_order_lines_table_order_id</t>
   </si>
   <si>
     <t>Reference to order</t>
   </si>
   <si>
-    <t>order_order_lines_item_id</t>
+    <t>order_order_lines_table_item_id</t>
   </si>
   <si>
     <t>Reference to item</t>
   </si>
   <si>
-    <t>order_items</t>
+    <t>order_items_table</t>
   </si>
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>order_order_lines_promotion_id</t>
-  </si>
-  <si>
-    <t>order_order_lines_segment_id</t>
-  </si>
-  <si>
-    <t>order_order_lines_business_area_id</t>
+    <t>order_order_lines_table_promotion_id</t>
+  </si>
+  <si>
+    <t>order_order_lines_table_segment_id</t>
+  </si>
+  <si>
+    <t>order_order_lines_table_business_area_id</t>
   </si>
   <si>
     <t>Analytic tables</t>

</xml_diff>